<commit_message>
add: WHED & required info if no WHED ID
</commit_message>
<xml_diff>
--- a/docs/files/Template_HEI_lists.xlsx
+++ b/docs/files/Template_HEI_lists.xlsx
@@ -20,8 +20,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Colin Tück</author>
+  </authors>
+  <commentList>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Fill in if the provider has another location different from the one specified in column L/M/N/O.
+If the provider has several other locations, please copy paste the columns Q, R, S, T, U and change the number in the brackets [n+1] for every next location.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The QF EHEA/EQF/ISCED level at which the provider offers programmes at.  Each new level should be presented in a new column with the subsequent number in brackets (i.e. [n+1]), i.e. put </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t xml:space="preserve">agency_id</t>
   </si>
@@ -41,6 +76,21 @@
     <t xml:space="preserve">acronym</t>
   </si>
   <si>
+    <t xml:space="preserve">identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifier_resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifier_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proof_of_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">local_identifier</t>
+  </si>
+  <si>
     <t xml:space="preserve">country_id</t>
   </si>
   <si>
@@ -50,6 +100,27 @@
     <t xml:space="preserve">postcode</t>
   </si>
   <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_location[1].country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_location[1].city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_location[1].postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_location[1].latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_location[1].longitude</t>
+  </si>
+  <si>
     <t xml:space="preserve">founding_date</t>
   </si>
   <si>
@@ -62,13 +133,16 @@
     <t xml:space="preserve">remarks_on_closing_date</t>
   </si>
   <si>
-    <t xml:space="preserve">qf_ehea_levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier_resource</t>
+    <t xml:space="preserve">qf_ehea_level[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qf_ehea_level[2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qf_ehea_level[3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qf_ehea_level[4]</t>
   </si>
   <si>
     <t xml:space="preserve">parent_id</t>
@@ -117,6 +191,98 @@
   <si>
     <r>
       <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Institution:
+identifier of this institution – </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">please provide WHED identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> if possible, e.g. IAU-123456</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution:
+type of the identifier (default: WHED)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Institution: 
+details on the source and issuer of the identifier – </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">required if this type is not yet known to EQAR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – skip for WHED</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Institution:
+official source (e.g. ministry website, national register, …) proving that this provider has full degree awarding powers in at least one higher education system – </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">required if no WHED identifier provided</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – institution's own website is not accepted</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution:
+Local identifier used for this institution by your agency</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -134,26 +300,37 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Institution legal seat:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">City</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Institution legal seat: postcode(include alphabets if any)</t>
+    <t xml:space="preserve">Institution:
+City of legal seat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution: postcode of  legal seat (include alphabets if any)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution: latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institution: longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional location:
+Country as ISO 3166 (2-letter or 3-letter) code or numerical DEQAR ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional location:
+City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional location:
+Postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional location:
+Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional location:
+Longitude</t>
   </si>
   <si>
     <t xml:space="preserve">Institution:
@@ -173,13 +350,6 @@
 - 3 or 8 or third cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">Institution:
-(local) identifier used for this institution by your agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name of the identifier (if external to your agency)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parent institution:
 if the institution is part of another institution (e.g. as a faculty, independent unit, …) or a grouping that is also recorded in DEQAR or ETER
 (given as numerical or DEQARINST ID)</t>
@@ -188,13 +358,20 @@
     <t xml:space="preserve">Type of relationship with parent institution, one of the following codes:
 - 1: consortium
 - 2: faculty (only for ES &amp; HR)
-- 3: independent faculty or school</t>
+- 3: independent faculty or school
+- 5: franchise or validation partnership</t>
   </si>
   <si>
     <t xml:space="preserve">* required</t>
   </si>
   <si>
     <t xml:space="preserve">optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recommended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conditionally req.</t>
   </si>
   <si>
     <r>
@@ -246,6 +423,9 @@
   </si>
   <si>
     <t xml:space="preserve">name_version_transliterated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qf_ehea_levels</t>
   </si>
   <si>
     <t xml:space="preserve">new_identifier</t>
@@ -327,6 +507,9 @@
   </si>
   <si>
     <t xml:space="preserve">add additional (local) identifier for this institution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of the identifier (if external to your agency)</t>
   </si>
   <si>
     <t xml:space="preserve">Add link to parent institution (numerical ID)
@@ -346,7 +529,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -374,6 +557,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -452,7 +641,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,12 +702,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -724,10 +917,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL4"/>
+  <dimension ref="A1:BY4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -736,15 +929,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="0" width="13.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="11" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="17" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="30.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,52 +968,78 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
       <c r="AH1" s="5"/>
@@ -848,124 +1073,213 @@
       <c r="BJ1" s="5"/>
       <c r="BK1" s="5"/>
       <c r="BL1" s="5"/>
+      <c r="BM1" s="5"/>
+      <c r="BN1" s="5"/>
+      <c r="BO1" s="5"/>
+      <c r="BP1" s="5"/>
+      <c r="BQ1" s="5"/>
+      <c r="BR1" s="5"/>
+      <c r="BS1" s="5"/>
+      <c r="BT1" s="5"/>
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5"/>
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="5"/>
     </row>
-    <row r="2" customFormat="false" ht="86.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="115.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>37</v>
+        <v>59</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="4" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
-      <c r="G4" s="17"/>
+    <row r="4" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="Q4" s="0"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Z2:AC2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -973,6 +1287,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -999,7 +1314,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="19" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="20" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.7"/>
@@ -1009,16 +1324,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -1030,19 +1345,19 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>45</v>
+        <v>69</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>4</v>
@@ -1051,31 +1366,31 @@
         <v>5</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
@@ -1123,136 +1438,136 @@
     </row>
     <row r="2" customFormat="false" ht="137.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="S3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="W3" s="21" t="s">
-        <v>36</v>
+        <v>59</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>